<commit_message>
Pushing stuff after exam
</commit_message>
<xml_diff>
--- a/Fall 2015/Lectures/Lecture 1 LP Intro/BakeSale.xlsx
+++ b/Fall 2015/Lectures/Lecture 1 LP Intro/BakeSale.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="6160" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="14460" yWindow="6160" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sensitivity Report 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sensitivity Report 1" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -98,12 +98,6 @@
     <t>Worksheet: [BakeSale.xlsx]Sheet1</t>
   </si>
   <si>
-    <t>Report Created: 8/28/2015 11:42:04 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Variable Cells </t>
-  </si>
-  <si>
     <t>Cell</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t>$F$14</t>
+  </si>
+  <si>
+    <t>Report Created: 10/7/2015 12:24:08 PM</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
   </si>
 </sst>
 </file>
@@ -202,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,12 +218,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3366FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,10 +276,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -641,111 +635,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
+      <c r="A3" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" thickBot="1">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" thickBot="1">
       <c r="B8" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-15</v>
+      </c>
+      <c r="F9" s="4">
+        <v>30</v>
+      </c>
+      <c r="G9" s="4">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1">
+      <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>30</v>
-      </c>
-      <c r="G9" s="5">
-        <v>30</v>
-      </c>
-      <c r="H9" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1">
-      <c r="B10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="6">
-        <v>4</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
         <v>60</v>
       </c>
-      <c r="G10" s="6">
-        <v>60</v>
-      </c>
-      <c r="H10" s="6">
-        <v>30</v>
+      <c r="G10" s="5">
+        <v>1E+30</v>
+      </c>
+      <c r="H10" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16" thickBot="1">
@@ -757,134 +751,134 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" thickBot="1">
       <c r="B14" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="E14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="G14" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4">
+        <v>12</v>
+      </c>
+      <c r="H15" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
+        <v>30</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>63</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1E+30</v>
+      </c>
+      <c r="H16" s="4">
         <v>33</v>
       </c>
-      <c r="C15" s="5" t="s">
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="D15" s="5">
-        <v>20</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>8</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="16" thickBot="1">
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
         <v>10</v>
       </c>
-      <c r="F15" s="5">
-        <v>20</v>
-      </c>
-      <c r="G15" s="5">
-        <v>12</v>
-      </c>
-      <c r="H15" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="5">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5">
-        <v>63</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="G18" s="5">
         <v>1E+30</v>
       </c>
-      <c r="H16" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="5">
-        <v>8</v>
-      </c>
-      <c r="E17" s="5">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5">
-        <v>8</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="H17" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="16" thickBot="1">
-      <c r="B18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="6">
-        <v>8</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1E+30</v>
-      </c>
-      <c r="H18" s="6">
-        <v>2</v>
+      <c r="H18" s="5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -899,10 +893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H14"/>
+  <dimension ref="C4:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:G36"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -924,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:8">
@@ -935,14 +929,14 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="E8">
         <v>60</v>
       </c>
       <c r="F8" s="2">
         <f>SUMPRODUCT(D8:E8,D5:E5)</f>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:8">
@@ -955,14 +949,14 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <f>SUMPRODUCT(D11:E11,$D$5:$E$5)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -981,9 +975,9 @@
       <c r="E12">
         <v>6</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <f t="shared" ref="F12:F14" si="0">SUMPRODUCT(D12:E12,$D$5:$E$5)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -1002,9 +996,9 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -1023,15 +1017,21 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
       </c>
       <c r="H14">
         <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13">
+      <c r="M19">
+        <f>315-(8*45)</f>
+        <v>-45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>